<commit_message>
#1245 PMD Rule 위반 수정
Todolist PMD Rule 위반 수정
</commit_message>
<xml_diff>
--- a/Subject_Dir/ToDolist_Dir/Trashcan.xlsx
+++ b/Subject_Dir/ToDolist_Dir/Trashcan.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>과목</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>알고리즘</t>
+  </si>
+  <si>
+    <t>�Է����ּ���qq</t>
   </si>
 </sst>
 </file>
@@ -89,7 +95,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -135,6 +141,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>